<commit_message>
wrangling raw ipeds into dashboardable ipeds
</commit_message>
<xml_diff>
--- a/R/wihera/inst/extdata/ipeds_schemas.xlsx
+++ b/R/wihera/inst/extdata/ipeds_schemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matts\Documents\GitHub\wihera\R\wihera\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BB7DBB-BB4C-48F5-809F-8902F3FAD202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3B973E-B6E5-4CBE-BC79-83812692D1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{D736E6D7-DA04-4085-AC36-D552D791C167}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{D736E6D7-DA04-4085-AC36-D552D791C167}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="241">
   <si>
     <t>UNITID</t>
   </si>
@@ -684,6 +684,84 @@
   </si>
   <si>
     <t>Disc</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Two or more races</t>
+  </si>
+  <si>
+    <t>Nonresident alien</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>under 18</t>
+  </si>
+  <si>
+    <t>18-24</t>
+  </si>
+  <si>
+    <t>25-39</t>
+  </si>
+  <si>
+    <t>40 and above</t>
+  </si>
+  <si>
+    <t>Enrollment Status</t>
+  </si>
+  <si>
+    <t>Full-time</t>
+  </si>
+  <si>
+    <t>Part-time</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>Previous Fall</t>
+  </si>
+  <si>
+    <t>Returning</t>
+  </si>
+  <si>
+    <t>Entering Students</t>
   </si>
 </sst>
 </file>
@@ -733,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -743,6 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B32345-DA7D-4128-8C12-018E99873D7F}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,9 +1239,11 @@
     <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>188</v>
       </c>
@@ -1184,8 +1265,14 @@
       <c r="G1" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1208,7 +1295,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>20662</v>
       </c>
@@ -1231,7 +1318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>20661</v>
       </c>
@@ -1254,7 +1341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>22023</v>
       </c>
@@ -1277,7 +1364,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>20781</v>
       </c>
@@ -1299,8 +1386,14 @@
       <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>20736</v>
       </c>
@@ -1322,8 +1415,14 @@
       <c r="G7" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>20741</v>
       </c>
@@ -1345,8 +1444,14 @@
       <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>24176</v>
       </c>
@@ -1368,8 +1473,14 @@
       <c r="G9" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>24111</v>
       </c>
@@ -1391,8 +1502,14 @@
       <c r="G10" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>24116</v>
       </c>
@@ -1414,8 +1531,14 @@
       <c r="G11" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>24181</v>
       </c>
@@ -1437,8 +1560,14 @@
       <c r="G12" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>24121</v>
       </c>
@@ -1460,8 +1589,14 @@
       <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>24126</v>
       </c>
@@ -1483,8 +1618,14 @@
       <c r="G14" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>24186</v>
       </c>
@@ -1506,8 +1647,14 @@
       <c r="G15" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>24131</v>
       </c>
@@ -1529,8 +1676,14 @@
       <c r="G16" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>24136</v>
       </c>
@@ -1552,8 +1705,14 @@
       <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>24171</v>
       </c>
@@ -1575,8 +1734,14 @@
       <c r="G18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>24101</v>
       </c>
@@ -1598,8 +1763,14 @@
       <c r="G19" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>24106</v>
       </c>
@@ -1621,8 +1792,14 @@
       <c r="G20" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>24191</v>
       </c>
@@ -1644,8 +1821,14 @@
       <c r="G21" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>24141</v>
       </c>
@@ -1667,8 +1850,14 @@
       <c r="G22" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>24146</v>
       </c>
@@ -1690,8 +1879,14 @@
       <c r="G23" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>24196</v>
       </c>
@@ -1713,8 +1908,14 @@
       <c r="G24" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24151</v>
       </c>
@@ -1736,8 +1937,14 @@
       <c r="G25" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24156</v>
       </c>
@@ -1759,8 +1966,14 @@
       <c r="G26" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>24201</v>
       </c>
@@ -1782,8 +1995,14 @@
       <c r="G27" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>24161</v>
       </c>
@@ -1805,8 +2024,14 @@
       <c r="G28" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>24166</v>
       </c>
@@ -1828,8 +2053,14 @@
       <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>20776</v>
       </c>
@@ -1851,8 +2082,14 @@
       <c r="G30" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>20726</v>
       </c>
@@ -1874,8 +2111,14 @@
       <c r="G31" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>20731</v>
       </c>
@@ -1897,8 +2140,14 @@
       <c r="G32" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>20746</v>
       </c>
@@ -1920,8 +2169,14 @@
       <c r="G33" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>20666</v>
       </c>
@@ -1943,8 +2198,14 @@
       <c r="G34" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>20671</v>
       </c>
@@ -1966,23 +2227,52 @@
       <c r="G35" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="H35" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8601EB71-9502-465A-BCB5-68CBB09A407D}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>188</v>
       </c>
@@ -2004,8 +2294,17 @@
       <c r="G1" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2028,7 +2327,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>33201</v>
       </c>
@@ -2051,7 +2350,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>33205</v>
       </c>
@@ -2073,8 +2372,17 @@
       <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>33210</v>
       </c>
@@ -2096,8 +2404,13 @@
       <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>33215</v>
       </c>
@@ -2119,8 +2432,13 @@
       <c r="G6" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>33220</v>
       </c>
@@ -2142,8 +2460,13 @@
       <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>33225</v>
       </c>
@@ -2165,8 +2488,13 @@
       <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>33230</v>
       </c>
@@ -2188,8 +2516,13 @@
       <c r="G9" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>33235</v>
       </c>
@@ -2211,8 +2544,13 @@
       <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>33240</v>
       </c>
@@ -2234,8 +2572,13 @@
       <c r="G11" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>33245</v>
       </c>
@@ -2257,8 +2600,13 @@
       <c r="G12" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>33250</v>
       </c>
@@ -2280,8 +2628,13 @@
       <c r="G13" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>33255</v>
       </c>
@@ -2303,8 +2656,13 @@
       <c r="G14" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>33260</v>
       </c>
@@ -2326,8 +2684,13 @@
       <c r="G15" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>33265</v>
       </c>
@@ -2349,8 +2712,13 @@
       <c r="G16" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>33270</v>
       </c>
@@ -2372,8 +2740,13 @@
       <c r="G17" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>33275</v>
       </c>
@@ -2395,8 +2768,13 @@
       <c r="G18" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>33280</v>
       </c>
@@ -2418,8 +2796,13 @@
       <c r="G19" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>33285</v>
       </c>
@@ -2440,6 +2823,11 @@
       </c>
       <c r="G20" s="1" t="s">
         <v>98</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2449,10 +2837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9826F9-75E6-47A5-B364-E4BC8E32C868}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,9 +2852,11 @@
     <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="72.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>188</v>
       </c>
@@ -2488,8 +2878,14 @@
       <c r="G1" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2512,7 +2908,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>21001</v>
       </c>
@@ -2534,8 +2930,14 @@
       <c r="G3" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>21006</v>
       </c>
@@ -2558,7 +2960,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>21011</v>
       </c>
@@ -2581,7 +2983,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>21026</v>
       </c>
@@ -2603,8 +3005,9 @@
       <c r="G6" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>21031</v>
       </c>
@@ -2626,8 +3029,9 @@
       <c r="G7" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>21033</v>
       </c>
@@ -2649,8 +3053,9 @@
       <c r="G8" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>21036</v>
       </c>
@@ -2672,8 +3077,14 @@
       <c r="G9" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>21041</v>
       </c>
@@ -2695,8 +3106,14 @@
       <c r="G10" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>21016</v>
       </c>
@@ -2718,8 +3135,10 @@
       <c r="G11" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>21046</v>
       </c>
@@ -2741,8 +3160,9 @@
       <c r="G12" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>21051</v>
       </c>
@@ -2764,8 +3184,9 @@
       <c r="G13" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>21053</v>
       </c>
@@ -2787,8 +3208,9 @@
       <c r="G14" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>21056</v>
       </c>
@@ -2810,8 +3232,14 @@
       <c r="G15" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>21061</v>
       </c>
@@ -2833,8 +3261,14 @@
       <c r="G16" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>21021</v>
       </c>
@@ -2856,8 +3290,10 @@
       <c r="G17" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>24301</v>
       </c>
@@ -2879,60 +3315,63 @@
       <c r="G18" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
     </row>

</xml_diff>